<commit_message>
Added pitch based binning to fixed tilt calcs
</commit_message>
<xml_diff>
--- a/Studies/USMap_Doubleday_2024/SETUPS Description Complete.xlsx
+++ b/Studies/USMap_Doubleday_2024/SETUPS Description Complete.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayala\Documents\GitHub\InSPIRE\Studies\USMap_Doubleday_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tford\dev\InSPIRE\Studies\USMap_Doubleday_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB492949-150A-4AFB-B383-867D185116FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1E840B-FF39-4D73-A020-3C6662939F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,8 @@
     <author>tc={9BA182C5-51A6-44C4-BCA5-828D6AE315C2}</author>
     <author>tc={7E70317A-F7B8-4FB0-8AA2-4C11CA037D47}</author>
     <author>tc={E6DDF6EE-C02E-4808-9F3D-14AAEF7C2636}</author>
+    <author>tc={2905C271-28C6-4CBE-BD8B-C8ED60F4304D}</author>
+    <author>tc={20EEDFF8-42AB-4C7B-A02A-728702A1D09F}</author>
   </authors>
   <commentList>
     <comment ref="F36" authorId="0" shapeId="0" xr:uid="{1111A611-2419-474B-8843-ABFCD803EC98}">
@@ -89,12 +91,30 @@
     Based on specific site pitch, choose one of these bins</t>
       </text>
     </comment>
+    <comment ref="F63" authorId="5" shapeId="0" xr:uid="{2905C271-28C6-4CBE-BD8B-C8ED60F4304D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is inclusive (0 to 2 means ground blocks 0, 1 and 2)
+Reply:
+    Still starts at 0 though 😝</t>
+      </text>
+    </comment>
+    <comment ref="D64" authorId="6" shapeId="0" xr:uid="{20EEDFF8-42AB-4C7B-A02A-728702A1D09F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Based on specific site pitch, choose one of these bins</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="99">
   <si>
     <t>Scenario</t>
   </si>
@@ -405,6 +425,33 @@
   <si>
     <t>Other equations that assume % of spectra and tranasform units; varying if W or Wh</t>
   </si>
+  <si>
+    <t>PITCH BINS</t>
+  </si>
+  <si>
+    <t>3.8 &lt;= pitch &lt; 3.8492</t>
+  </si>
+  <si>
+    <t>3.8492 &lt;= pitch &lt;4.9491</t>
+  </si>
+  <si>
+    <t>4.9491 &lt;= pitch &lt; 6.9355</t>
+  </si>
+  <si>
+    <t>11.5465 &lt;= pitch &lt; 12</t>
+  </si>
+  <si>
+    <t>pitch resolution</t>
+  </si>
+  <si>
+    <t>6.9355 &lt;= pitch &lt; 11.5465</t>
+  </si>
+  <si>
+    <t>Fixed Tilts BINNED</t>
+  </si>
+  <si>
+    <t>calculated with 30 degrees tilt</t>
+  </si>
 </sst>
 </file>
 
@@ -413,7 +460,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +560,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -872,6 +925,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,25 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -948,13 +1001,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>752</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>133609</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1335,15 +1388,24 @@
   <threadedComment ref="D49" dT="2025-08-26T21:16:42.62" personId="{7239D7DF-F240-4F71-ABD2-13E2A2CDE475}" id="{E6DDF6EE-C02E-4808-9F3D-14AAEF7C2636}">
     <text>Based on specific site pitch, choose one of these bins</text>
   </threadedComment>
+  <threadedComment ref="F63" dT="2025-08-26T20:46:04.80" personId="{7239D7DF-F240-4F71-ABD2-13E2A2CDE475}" id="{2905C271-28C6-4CBE-BD8B-C8ED60F4304D}">
+    <text>This is inclusive (0 to 2 means ground blocks 0, 1 and 2)</text>
+  </threadedComment>
+  <threadedComment ref="F63" dT="2025-08-26T21:20:41.65" personId="{7239D7DF-F240-4F71-ABD2-13E2A2CDE475}" id="{46181303-F1FB-4AE7-89D7-9C730F5FE5C5}" parentId="{2905C271-28C6-4CBE-BD8B-C8ED60F4304D}">
+    <text>Still starts at 0 though 😝</text>
+  </threadedComment>
+  <threadedComment ref="D64" dT="2025-08-26T21:16:42.62" personId="{7239D7DF-F240-4F71-ABD2-13E2A2CDE475}" id="{20EEDFF8-42AB-4C7B-A02A-728702A1D09F}">
+    <text>Based on specific site pitch, choose one of these bins</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A1107-9899-4DFE-A9E6-0ED2844D3F4A}">
-  <dimension ref="B2:AA84"/>
+  <dimension ref="B2:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="C50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,10 +1427,10 @@
       <c r="B2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="67" t="s">
+      <c r="T2" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="67"/>
+      <c r="U2" s="73"/>
     </row>
     <row r="3" spans="2:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
@@ -2157,23 +2219,23 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="68" t="s">
+      <c r="G26" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>3.8</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="71"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -2183,16 +2245,16 @@
         <v>2</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>34</v>
@@ -2203,9 +2265,9 @@
       <c r="F29" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="70"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -2213,25 +2275,25 @@
       </c>
       <c r="C30">
         <f>C28*COS(RADIANS(C29))</f>
-        <v>2</v>
+        <v>1.7320508075688774</v>
       </c>
       <c r="D30">
         <f>C30*100/C27</f>
-        <v>25</v>
+        <v>45.580284409707303</v>
       </c>
       <c r="E30">
         <f>D30/10</f>
-        <v>2.5</v>
+        <v>4.5580284409707303</v>
       </c>
       <c r="F30" s="6">
         <f>ROUND(D30/10,0)</f>
-        <v>3</v>
-      </c>
-      <c r="G30" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
     </row>
     <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
@@ -2239,60 +2301,60 @@
       </c>
       <c r="C31" s="10">
         <f>C27-C30</f>
-        <v>6</v>
+        <v>2.0679491924311222</v>
       </c>
       <c r="D31" s="10">
         <f>C31*100/C27</f>
-        <v>75</v>
+        <v>54.419715590292689</v>
       </c>
       <c r="E31" s="10">
         <f>D31/10</f>
-        <v>7.5</v>
+        <v>5.4419715590292688</v>
       </c>
       <c r="F31" s="11">
         <f>ROUND(D31/10,0)</f>
-        <v>8</v>
-      </c>
-      <c r="G31" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
     </row>
     <row r="35" spans="3:25" x14ac:dyDescent="0.25">
       <c r="O35"/>
     </row>
     <row r="36" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="73"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="36"/>
       <c r="E36" s="36"/>
-      <c r="F36" s="72" t="s">
+      <c r="F36" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="73" t="s">
+      <c r="G36" s="77"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="73"/>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="73"/>
-      <c r="S36" s="73"/>
-      <c r="T36" s="73"/>
-      <c r="U36" s="73"/>
-      <c r="V36" s="73"/>
-      <c r="W36" s="73"/>
-      <c r="X36" s="73"/>
-      <c r="Y36" s="73"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="62"/>
+      <c r="T36" s="62"/>
+      <c r="U36" s="62"/>
+      <c r="V36" s="62"/>
+      <c r="W36" s="62"/>
+      <c r="X36" s="62"/>
+      <c r="Y36" s="62"/>
     </row>
     <row r="37" spans="3:25" s="37" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="73"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="38" t="s">
         <v>0</v>
       </c>
@@ -2361,7 +2423,7 @@
       </c>
     </row>
     <row r="38" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C38" s="74" t="s">
+      <c r="C38" s="63" t="s">
         <v>66</v>
       </c>
       <c r="D38">
@@ -2414,7 +2476,7 @@
       </c>
     </row>
     <row r="39" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C39" s="74"/>
+      <c r="C39" s="63"/>
       <c r="D39">
         <v>2</v>
       </c>
@@ -2465,7 +2527,7 @@
       </c>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C40" s="74"/>
+      <c r="C40" s="63"/>
       <c r="D40">
         <v>3</v>
       </c>
@@ -2516,7 +2578,7 @@
       </c>
     </row>
     <row r="41" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C41" s="74"/>
+      <c r="C41" s="63"/>
       <c r="D41">
         <v>4</v>
       </c>
@@ -2567,7 +2629,7 @@
       </c>
     </row>
     <row r="42" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C42" s="74"/>
+      <c r="C42" s="63"/>
       <c r="D42">
         <v>5</v>
       </c>
@@ -2723,38 +2785,38 @@
       <c r="O47"/>
     </row>
     <row r="48" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="75" t="s">
+      <c r="C48" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="D48" s="77" t="s">
+      <c r="D48" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="E48" s="77"/>
-      <c r="F48" s="72" t="s">
+      <c r="E48" s="66"/>
+      <c r="F48" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="G48" s="72"/>
-      <c r="H48" s="72"/>
-      <c r="I48" s="72"/>
-      <c r="J48" s="73" t="s">
+      <c r="G48" s="77"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77"/>
+      <c r="J48" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K48" s="73"/>
-      <c r="L48" s="73"/>
-      <c r="M48" s="73"/>
-      <c r="N48" s="73"/>
-      <c r="O48" s="73"/>
-      <c r="P48" s="73"/>
-      <c r="Q48" s="73"/>
-      <c r="R48" s="73"/>
-      <c r="S48" s="73"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="62"/>
+      <c r="M48" s="62"/>
+      <c r="N48" s="62"/>
+      <c r="O48" s="62"/>
+      <c r="P48" s="62"/>
+      <c r="Q48" s="62"/>
+      <c r="R48" s="62"/>
+      <c r="S48" s="62"/>
     </row>
     <row r="49" spans="3:19" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="75"/>
-      <c r="D49" s="76" t="s">
+      <c r="C49" s="64"/>
+      <c r="D49" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="E49" s="76"/>
+      <c r="E49" s="65"/>
       <c r="F49" s="39" t="s">
         <v>57</v>
       </c>
@@ -2799,11 +2861,11 @@
       </c>
     </row>
     <row r="50" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C50" s="75"/>
-      <c r="D50" s="71">
+      <c r="C50" s="64"/>
+      <c r="D50" s="67">
         <v>3.8</v>
       </c>
-      <c r="E50" s="71"/>
+      <c r="E50" s="67"/>
       <c r="F50">
         <v>0</v>
       </c>
@@ -2848,11 +2910,11 @@
       </c>
     </row>
     <row r="51" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C51" s="75"/>
-      <c r="D51" s="71">
+      <c r="C51" s="64"/>
+      <c r="D51" s="67">
         <v>4</v>
       </c>
-      <c r="E51" s="71"/>
+      <c r="E51" s="67"/>
       <c r="F51">
         <v>0</v>
       </c>
@@ -2897,11 +2959,11 @@
       </c>
     </row>
     <row r="52" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C52" s="75"/>
-      <c r="D52" s="71">
+      <c r="C52" s="64"/>
+      <c r="D52" s="67">
         <v>4.5</v>
       </c>
-      <c r="E52" s="71"/>
+      <c r="E52" s="67"/>
       <c r="F52">
         <v>0</v>
       </c>
@@ -2946,11 +3008,11 @@
       </c>
     </row>
     <row r="53" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C53" s="75"/>
-      <c r="D53" s="71">
+      <c r="C53" s="64"/>
+      <c r="D53" s="67">
         <v>5</v>
       </c>
-      <c r="E53" s="71"/>
+      <c r="E53" s="67"/>
       <c r="F53">
         <v>0</v>
       </c>
@@ -2995,11 +3057,11 @@
       </c>
     </row>
     <row r="54" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C54" s="75"/>
-      <c r="D54" s="71">
+      <c r="C54" s="64"/>
+      <c r="D54" s="67">
         <v>5.5</v>
       </c>
-      <c r="E54" s="71"/>
+      <c r="E54" s="67"/>
       <c r="F54">
         <v>0</v>
       </c>
@@ -3044,11 +3106,11 @@
       </c>
     </row>
     <row r="55" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C55" s="75"/>
-      <c r="D55" s="71">
+      <c r="C55" s="64"/>
+      <c r="D55" s="67">
         <v>6</v>
       </c>
-      <c r="E55" s="71"/>
+      <c r="E55" s="67"/>
       <c r="F55">
         <v>0</v>
       </c>
@@ -3093,11 +3155,11 @@
       </c>
     </row>
     <row r="56" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C56" s="75"/>
-      <c r="D56" s="71">
+      <c r="C56" s="64"/>
+      <c r="D56" s="67">
         <v>6.5</v>
       </c>
-      <c r="E56" s="71"/>
+      <c r="E56" s="67"/>
       <c r="F56">
         <v>0</v>
       </c>
@@ -3142,11 +3204,11 @@
       </c>
     </row>
     <row r="57" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C57" s="75"/>
-      <c r="D57" s="71">
+      <c r="C57" s="64"/>
+      <c r="D57" s="67">
         <v>7</v>
       </c>
-      <c r="E57" s="71"/>
+      <c r="E57" s="67"/>
       <c r="F57">
         <v>0</v>
       </c>
@@ -3191,11 +3253,11 @@
       </c>
     </row>
     <row r="58" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C58" s="75"/>
-      <c r="D58" s="71">
+      <c r="C58" s="64"/>
+      <c r="D58" s="67">
         <v>7.5</v>
       </c>
-      <c r="E58" s="71"/>
+      <c r="E58" s="67"/>
       <c r="F58">
         <v>0</v>
       </c>
@@ -3240,11 +3302,11 @@
       </c>
     </row>
     <row r="59" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C59" s="75"/>
-      <c r="D59" s="71">
+      <c r="C59" s="64"/>
+      <c r="D59" s="67">
         <v>8</v>
       </c>
-      <c r="E59" s="71"/>
+      <c r="E59" s="67"/>
       <c r="F59">
         <v>0</v>
       </c>
@@ -3289,11 +3351,11 @@
       </c>
     </row>
     <row r="60" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C60" s="75"/>
-      <c r="D60" s="71">
+      <c r="C60" s="64"/>
+      <c r="D60" s="67">
         <v>8.5</v>
       </c>
-      <c r="E60" s="71"/>
+      <c r="E60" s="67"/>
       <c r="F60">
         <v>0</v>
       </c>
@@ -3338,11 +3400,11 @@
       </c>
     </row>
     <row r="61" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C61" s="75"/>
-      <c r="D61" s="71">
+      <c r="C61" s="64"/>
+      <c r="D61" s="67">
         <v>9</v>
       </c>
-      <c r="E61" s="71"/>
+      <c r="E61" s="67"/>
       <c r="F61">
         <v>0</v>
       </c>
@@ -3390,220 +3452,629 @@
       <c r="D62" t="s">
         <v>64</v>
       </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-      <c r="G62">
+      <c r="M62" s="1"/>
+      <c r="O62"/>
+    </row>
+    <row r="63" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E63" s="66"/>
+      <c r="F63" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="G63" s="77"/>
+      <c r="H63" s="77"/>
+      <c r="I63" s="77"/>
+      <c r="J63" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="K63" s="62"/>
+      <c r="L63" s="62"/>
+      <c r="M63" s="62"/>
+      <c r="N63" s="62"/>
+      <c r="O63" s="62"/>
+      <c r="P63" s="62"/>
+      <c r="Q63" s="62"/>
+      <c r="R63" s="62"/>
+      <c r="S63" s="62"/>
+    </row>
+    <row r="64" spans="3:19" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="64"/>
+      <c r="D64" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="E64" s="65"/>
+      <c r="F64" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G64" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H64" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="I64" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="J64" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K64" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="L64" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="M64" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="N64" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="O64" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="P64" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q64" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="R64" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="S64" s="45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C65" s="64"/>
+      <c r="D65" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" s="67"/>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>45</v>
+      </c>
+      <c r="I65" t="s">
+        <v>45</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>5</v>
+      </c>
+      <c r="L65" t="s">
+        <v>45</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N65">
+        <v>5</v>
+      </c>
+      <c r="O65">
+        <v>7</v>
+      </c>
+      <c r="P65">
+        <v>7</v>
+      </c>
+      <c r="Q65">
+        <v>8</v>
+      </c>
+      <c r="R65">
+        <v>8</v>
+      </c>
+      <c r="S65" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA65" s="1"/>
+    </row>
+    <row r="66" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C66" s="64"/>
+      <c r="D66" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="E66" s="67"/>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66" t="s">
+        <v>45</v>
+      </c>
+      <c r="I66" t="s">
+        <v>45</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>4</v>
+      </c>
+      <c r="L66" t="s">
+        <v>45</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N66">
+        <v>4</v>
+      </c>
+      <c r="O66">
+        <v>6</v>
+      </c>
+      <c r="P66">
+        <v>6</v>
+      </c>
+      <c r="Q66">
+        <v>8</v>
+      </c>
+      <c r="R66">
+        <v>8</v>
+      </c>
+      <c r="S66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C67" s="64"/>
+      <c r="D67" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="E67" s="67"/>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67" t="s">
+        <v>45</v>
+      </c>
+      <c r="I67" t="s">
+        <v>45</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>3</v>
+      </c>
+      <c r="L67" t="s">
+        <v>45</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N67">
+        <v>3</v>
+      </c>
+      <c r="O67">
+        <v>5</v>
+      </c>
+      <c r="P67">
+        <v>5</v>
+      </c>
+      <c r="Q67">
+        <v>8</v>
+      </c>
+      <c r="R67">
+        <v>8</v>
+      </c>
+      <c r="S67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C68" s="64"/>
+      <c r="D68" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="E68" s="67"/>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
         <v>1</v>
       </c>
-      <c r="H62" t="s">
-        <v>45</v>
-      </c>
-      <c r="I62" t="s">
-        <v>45</v>
-      </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
+      <c r="H68" t="s">
+        <v>45</v>
+      </c>
+      <c r="I68" t="s">
+        <v>45</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>2</v>
+      </c>
+      <c r="L68" t="s">
+        <v>45</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N68">
+        <v>2</v>
+      </c>
+      <c r="O68">
+        <v>5</v>
+      </c>
+      <c r="P68">
+        <v>5</v>
+      </c>
+      <c r="Q68">
+        <v>7</v>
+      </c>
+      <c r="R68">
+        <v>7</v>
+      </c>
+      <c r="S68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C69" s="64"/>
+      <c r="D69" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" s="67"/>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69" t="s">
+        <v>45</v>
+      </c>
+      <c r="I69" t="s">
+        <v>45</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
         <v>1</v>
       </c>
-      <c r="L62" t="s">
-        <v>45</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N62">
+      <c r="L69" t="s">
+        <v>45</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N69">
         <v>1</v>
       </c>
-      <c r="O62">
+      <c r="O69">
         <v>4</v>
       </c>
-      <c r="P62">
+      <c r="P69">
         <v>4</v>
       </c>
-      <c r="Q62">
+      <c r="Q69">
         <v>7</v>
       </c>
-      <c r="R62">
+      <c r="R69">
         <v>7</v>
       </c>
-      <c r="S62" t="s">
+      <c r="S69" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="M63" s="1"/>
-      <c r="O63"/>
-    </row>
-    <row r="64" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N64" s="1"/>
-      <c r="O64"/>
-    </row>
-    <row r="65" spans="3:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C65" s="55" t="s">
+    <row r="70" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C70" s="64"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="67"/>
+      <c r="M70" s="1"/>
+      <c r="O70"/>
+    </row>
+    <row r="71" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C71" s="64"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="67"/>
+      <c r="M71" s="1"/>
+      <c r="O71"/>
+    </row>
+    <row r="72" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C72" s="64"/>
+      <c r="D72" s="67"/>
+      <c r="E72" s="67"/>
+      <c r="M72" s="1"/>
+      <c r="O72"/>
+    </row>
+    <row r="73" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C73" s="64"/>
+    </row>
+    <row r="74" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C74" s="64"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="67"/>
+      <c r="M74" s="1"/>
+      <c r="O74"/>
+    </row>
+    <row r="75" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C75" s="64"/>
+      <c r="D75" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="E75" s="67"/>
+      <c r="M75" s="1"/>
+      <c r="O75"/>
+    </row>
+    <row r="76" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C76" s="64"/>
+      <c r="D76">
+        <f>8.2/1000</f>
+        <v>8.199999999999999E-3</v>
+      </c>
+      <c r="E76" t="s">
+        <v>95</v>
+      </c>
+      <c r="M76" s="1"/>
+      <c r="O76"/>
+    </row>
+    <row r="79" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="3:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C80" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="D65" s="56"/>
-      <c r="E65" s="57"/>
-      <c r="O65"/>
-      <c r="AA65" s="1"/>
-    </row>
-    <row r="66" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C66" s="5" t="s">
+      <c r="D80" s="56"/>
+      <c r="E80" s="57"/>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E66" s="59"/>
-    </row>
-    <row r="67" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C67" s="5" t="s">
+      <c r="E81" s="59"/>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C82" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="52">
-        <f>F67*0.3048</f>
+      <c r="D82" s="52">
+        <f>F82*0.3048</f>
         <v>0.15240000000000001</v>
       </c>
-      <c r="E67" s="59" t="s">
+      <c r="E82" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="F67">
+      <c r="F82">
         <v>0.5</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G82" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C68" s="5" t="s">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C83" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="52">
+      <c r="D83" s="52">
         <v>5</v>
       </c>
-      <c r="E68" s="59" t="s">
+      <c r="E83" s="59" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C69" s="5" t="s">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D69" s="52">
+      <c r="D84" s="52">
         <v>2</v>
       </c>
-      <c r="E69" s="59" t="s">
+      <c r="E84" s="59" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C70" s="5" t="s">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70" s="59" t="s">
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85" s="59" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C71" s="5" t="s">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D71">
-        <f>D69/D68</f>
+      <c r="D86">
+        <f>D84/D83</f>
         <v>0.4</v>
       </c>
-      <c r="E71" s="59"/>
-    </row>
-    <row r="72" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C72" s="5" t="s">
+      <c r="E86" s="59"/>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D72">
-        <f>D69*COS(RADIANS(D70))</f>
+      <c r="D87">
+        <f>D84*COS(RADIANS(D85))</f>
         <v>2</v>
       </c>
-      <c r="E72" s="61" t="s">
+      <c r="E87" s="61" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C73" s="5" t="s">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D73">
-        <f>D68-D72</f>
+      <c r="D88">
+        <f>D83-D87</f>
         <v>3</v>
       </c>
-      <c r="E73" s="59" t="s">
+      <c r="E88" s="59" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C74" s="5" t="s">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C89" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D74">
-        <f>D73-2*D67</f>
+      <c r="D89">
+        <f>D88-2*D82</f>
         <v>2.6951999999999998</v>
       </c>
-      <c r="E74" s="59" t="s">
+      <c r="E89" s="59" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C75" s="53" t="s">
+    <row r="90" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="54">
-        <f>D74*100/D68</f>
+      <c r="D90" s="54">
+        <f>D89*100/D83</f>
         <v>53.903999999999996</v>
       </c>
-      <c r="E75" s="60" t="s">
+      <c r="E90" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="3:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C79" s="64" t="s">
+    <row r="93" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C94" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="D79" s="65"/>
-      <c r="E79" s="66"/>
-    </row>
-    <row r="80" spans="3:27" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C80" s="9" t="s">
+      <c r="D94" s="71"/>
+      <c r="E94" s="72"/>
+    </row>
+    <row r="95" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D80" s="58" t="s">
+      <c r="D95" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="E80" s="11" t="s">
+      <c r="E95" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C82" s="7" t="s">
+    <row r="97" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C97" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
+    <row r="98" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+    <row r="99" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
         <v>87</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E99" t="s">
         <v>83</v>
       </c>
     </row>
+    <row r="100" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O100"/>
+    </row>
+    <row r="101" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O101"/>
+    </row>
+    <row r="102" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O102"/>
+    </row>
+    <row r="103" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O103"/>
+    </row>
+    <row r="104" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O104"/>
+    </row>
+    <row r="105" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O105"/>
+    </row>
+    <row r="106" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O106"/>
+    </row>
+    <row r="107" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O107"/>
+    </row>
+    <row r="108" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O108"/>
+    </row>
+    <row r="109" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O109"/>
+    </row>
+    <row r="110" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O110"/>
+    </row>
+    <row r="111" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O111"/>
+    </row>
+    <row r="112" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O112"/>
+    </row>
+    <row r="113" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="O113"/>
+    </row>
+    <row r="114" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="O114"/>
+    </row>
+    <row r="115" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M115" s="1"/>
+      <c r="O115"/>
+    </row>
+    <row r="116" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M116" s="1"/>
+      <c r="O116"/>
+    </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="44">
+    <mergeCell ref="C63:C76"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="J63:S63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="J36:Y36"/>
     <mergeCell ref="J48:S48"/>
     <mergeCell ref="C38:C42"/>
     <mergeCell ref="C48:C61"/>
@@ -3617,22 +4088,6 @@
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="J36:Y36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>